<commit_message>
All records for 1000 datapoints and some for 2000 for PointNet, hier hdbscan dbcv scores for Conclu
</commit_message>
<xml_diff>
--- a/Experiments/DBCV_Conclu.xlsx
+++ b/Experiments/DBCV_Conclu.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="195">
   <si>
     <t>Datapoints</t>
   </si>
@@ -580,6 +580,39 @@
   </si>
   <si>
     <t>126.927 secs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 1 </t>
+  </si>
+  <si>
+    <t>298 clusters</t>
+  </si>
+  <si>
+    <t>95 outliers</t>
+  </si>
+  <si>
+    <t>0.141</t>
+  </si>
+  <si>
+    <t>225.495 secs</t>
+  </si>
+  <si>
+    <t>Algo</t>
+  </si>
+  <si>
+    <t>no. Of clusters</t>
+  </si>
+  <si>
+    <t>Outliers</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>-0.095</t>
+  </si>
+  <si>
+    <t>56.624 secs</t>
   </si>
 </sst>
 </file>
@@ -650,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -668,6 +701,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,10 +1012,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1008,32 +1047,32 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="I4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="J4" s="8" t="s">
         <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>10</v>
@@ -1052,28 +1091,28 @@
       <c r="A5" s="3">
         <v>1000</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3">
+        <v>512</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3">
+      <c r="I5" s="3">
         <v>303</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="J5" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="3">
-        <v>512</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3">
-        <v>2</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>18</v>
@@ -1088,29 +1127,29 @@
       <c r="A6" s="3">
         <v>1000</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3">
+        <v>512</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3">
+        <v>154</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3">
+      <c r="I6" s="3">
         <v>169</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3">
-        <v>512</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="3">
-        <v>154</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1124,29 +1163,29 @@
       <c r="A7" s="3">
         <v>1000</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3">
+        <v>512</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3">
+        <v>154</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3">
+      <c r="I7" s="3">
         <v>175</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="J7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3">
-        <v>512</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="3">
-        <v>154</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1160,28 +1199,28 @@
       <c r="A8" s="3">
         <v>1000</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3">
+        <v>512</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="3">
+      <c r="I8" s="3">
         <v>175</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="J8" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="3">
-        <v>512</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3">
-        <v>2</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>34</v>
@@ -1196,28 +1235,28 @@
       <c r="A9" s="3">
         <v>1000</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3">
+        <v>512</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3">
+      <c r="I9" s="3">
         <v>175</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="J9" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" s="3">
-        <v>512</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3">
-        <v>2</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>40</v>
@@ -1232,29 +1271,29 @@
       <c r="A10" s="3">
         <v>1000</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3">
+        <v>512</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3">
+        <v>154</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3">
+      <c r="I10" s="3">
         <v>175</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="J10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="3">
-        <v>512</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="3">
-        <v>154</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1268,29 +1307,29 @@
       <c r="A11" s="3">
         <v>1000</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3">
+        <v>512</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3">
+        <v>154</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="3">
+      <c r="I11" s="3">
         <v>175</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="J11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="3">
-        <v>512</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="3">
-        <v>154</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="2"/>
       <c r="K11" s="4" t="s">
         <v>51</v>
       </c>
@@ -1308,28 +1347,28 @@
       <c r="A12" s="3">
         <v>1000</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3">
+        <v>512</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="3">
+      <c r="I12" s="3">
         <v>175</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="J12" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="E12" s="3">
-        <v>512</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3">
-        <v>2</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>57</v>
@@ -1342,15 +1381,12 @@
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1358,15 +1394,12 @@
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1376,28 +1409,28 @@
       <c r="A15" s="3">
         <v>2000</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3">
+        <v>512</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="3">
+      <c r="I15" s="3">
         <v>175</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="J15" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="E15" s="3">
-        <v>512</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>62</v>
@@ -1412,29 +1445,29 @@
       <c r="A16" s="3">
         <v>2000</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3">
+        <v>512</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="3">
+        <v>154</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3">
+      <c r="I16" s="3">
         <v>175</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="J16" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="3">
-        <v>512</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="3">
-        <v>154</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
         <v>67</v>
       </c>
@@ -1448,29 +1481,29 @@
       <c r="A17" s="3">
         <v>2000</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3">
+        <v>512</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="3">
+        <v>154</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1">
+      <c r="I17" s="7">
         <v>175</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="3">
-        <v>512</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G17" s="3">
-        <v>154</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="2"/>
       <c r="K17" s="6" t="s">
         <v>139</v>
       </c>
@@ -1486,28 +1519,28 @@
       <c r="A18" s="3">
         <v>2000</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3">
+        <v>512</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="3">
+      <c r="I18" s="3">
         <v>175</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="J18" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="E18" s="3">
-        <v>512</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3">
-        <v>2</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>73</v>
@@ -1522,29 +1555,29 @@
       <c r="A19" s="3">
         <v>2000</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3">
+        <v>512</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="3">
+        <v>154</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3">
+      <c r="I19" s="3">
         <v>363</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="J19" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="3">
-        <v>512</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="3">
-        <v>154</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
         <v>78</v>
       </c>
@@ -1558,28 +1591,28 @@
       <c r="A20" s="3">
         <v>2000</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3">
+        <v>512</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="3">
+      <c r="I20" s="3">
         <v>605</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="J20" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E20" s="3">
-        <v>512</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3">
-        <v>2</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>83</v>
@@ -1594,29 +1627,29 @@
       <c r="A21" s="3">
         <v>2000</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3">
+        <v>512</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="3">
+        <v>154</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="3">
+      <c r="I21" s="3">
         <v>175</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="J21" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="3">
-        <v>512</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="3">
-        <v>154</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
         <v>88</v>
       </c>
@@ -1630,28 +1663,28 @@
       <c r="A22" s="3">
         <v>2000</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3">
+        <v>512</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="3">
+      <c r="I22" s="3">
         <v>175</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="J22" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="E22" s="3">
-        <v>512</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="3">
-        <v>2</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>93</v>
@@ -1664,15 +1697,12 @@
     </row>
     <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1680,15 +1710,12 @@
     </row>
     <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -1698,28 +1725,28 @@
       <c r="A25" s="3">
         <v>5000</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3">
+        <v>512</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="3">
+      <c r="I25" s="3">
         <v>1586</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="J25" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="E25" s="3">
-        <v>512</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="3">
-        <v>2</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>117</v>
@@ -1734,29 +1761,29 @@
       <c r="A26" s="1">
         <v>5000</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="1">
+        <v>512</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="1">
+        <v>154</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="1">
+      <c r="I26" s="7">
         <v>914</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="J26" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E26" s="1">
-        <v>512</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="G26" s="1">
-        <v>154</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="2"/>
       <c r="K26" s="6" t="s">
         <v>125</v>
       </c>
@@ -1772,28 +1799,28 @@
       <c r="A27" s="3">
         <v>5000</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3">
+        <v>512</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3">
+        <v>2</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="3">
+      <c r="I27" s="3">
         <v>175</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="J27" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="E27" s="3">
-        <v>512</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="3">
-        <v>2</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>103</v>
@@ -1808,29 +1835,29 @@
       <c r="A28" s="1">
         <v>5000</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="1">
+        <v>512</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="1">
+        <v>154</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="1">
+      <c r="I28" s="7">
         <v>175</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="J28" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E28" s="1">
-        <v>512</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G28" s="1">
-        <v>154</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
         <v>107</v>
       </c>
@@ -1846,28 +1873,28 @@
       <c r="A29" s="1">
         <v>5000</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="1">
+        <v>512</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="1">
+      <c r="I29" s="7">
         <v>175</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="J29" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="E29" s="1">
-        <v>512</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="1">
-        <v>2</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="K29" s="6" t="s">
         <v>113</v>
@@ -1882,29 +1909,29 @@
       <c r="A30" s="1">
         <v>5000</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="1">
+        <v>512</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="1">
+        <v>154</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="1">
+      <c r="I30" s="7">
         <v>175</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="J30" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="1">
-        <v>512</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G30" s="1">
-        <v>154</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="2"/>
       <c r="K30" s="6" t="s">
         <v>120</v>
       </c>
@@ -1922,28 +1949,28 @@
       <c r="A31" s="1">
         <v>5000</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="1">
+        <v>512</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="1">
+      <c r="I31" s="7">
         <v>175</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="J31" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="E31" s="1">
-        <v>512</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="1">
-        <v>2</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>130</v>
@@ -1958,29 +1985,29 @@
       <c r="A32" s="1">
         <v>5000</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="1">
+        <v>512</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="1">
+        <v>154</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="1">
+      <c r="I32" s="7">
         <v>175</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="J32" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E32" s="1">
-        <v>512</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="G32" s="1">
-        <v>154</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="2"/>
       <c r="K32" s="6" t="s">
         <v>151</v>
       </c>
@@ -2057,52 +2084,51 @@
       <c r="N36" s="2"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="G37" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="B37" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A38" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="B38" s="8" t="s">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>3</v>
+        <v>191</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L38" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
@@ -2112,259 +2138,347 @@
       <c r="B39" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="8">
+        <v>76</v>
+      </c>
+      <c r="I39" s="7">
+        <v>48</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G54" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L55" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M55" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N55" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A56" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="7">
         <v>165</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D56" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E39" s="7">
-        <v>512</v>
-      </c>
-      <c r="F39" s="8" t="s">
+      <c r="E56" s="7">
+        <v>512</v>
+      </c>
+      <c r="F56" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G56" s="7">
         <v>154</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H56" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="K39" s="6" t="s">
+      <c r="K56" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="L56" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A40" s="7">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A57" s="7">
         <v>1000</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B57" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C57" s="7">
         <v>323</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D57" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E40" s="7">
-        <v>512</v>
-      </c>
-      <c r="F40" s="8" t="s">
+      <c r="E57" s="7">
+        <v>512</v>
+      </c>
+      <c r="F57" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I40" s="7">
+      <c r="I57" s="7">
         <v>2</v>
       </c>
-      <c r="J40" s="8" t="s">
+      <c r="J57" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="K40" s="8" t="s">
+      <c r="K57" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="L40" s="8" t="s">
+      <c r="L57" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A41" s="7">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A58" s="7">
         <v>1000</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B58" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C58" s="7">
         <v>175</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D58" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E41" s="7">
-        <v>512</v>
-      </c>
-      <c r="F41" s="8" t="s">
+      <c r="E58" s="7">
+        <v>512</v>
+      </c>
+      <c r="F58" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="I41" s="7">
+      <c r="I58" s="7">
         <v>2</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="J58" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="K41" s="6" t="s">
+      <c r="K58" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="L41" s="8" t="s">
+      <c r="L58" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A42" s="7">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A59" s="7">
         <v>1000</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B59" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C59" s="7">
         <v>175</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D59" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="7">
-        <v>512</v>
-      </c>
-      <c r="F42" s="8" t="s">
+      <c r="E59" s="7">
+        <v>512</v>
+      </c>
+      <c r="F59" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G59" s="7">
         <v>154</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H59" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="K42" s="6" t="s">
+      <c r="K59" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="L42" s="8" t="s">
+      <c r="L59" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="N42" s="8" t="s">
+      <c r="N59" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A43" s="7">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A60" s="7">
         <v>1000</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B60" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C60" s="7">
         <v>175</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D60" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E43" s="7">
-        <v>512</v>
-      </c>
-      <c r="F43" s="8" t="s">
+      <c r="E60" s="7">
+        <v>512</v>
+      </c>
+      <c r="F60" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="I43" s="7">
+      <c r="I60" s="7">
         <v>2</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="J60" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="K43" s="6" t="s">
+      <c r="K60" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="L43" s="8" t="s">
+      <c r="L60" s="8" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A44" s="7">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A61" s="7">
         <v>1000</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C61" s="7">
         <v>175</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D61" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E44" s="7">
-        <v>512</v>
-      </c>
-      <c r="F44" s="8" t="s">
+      <c r="E61" s="7">
+        <v>512</v>
+      </c>
+      <c r="F61" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G61" s="7">
         <v>154</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H61" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="K44" s="6" t="s">
+      <c r="K61" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="L44" s="8" t="s">
+      <c r="L61" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A45" s="7">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A62" s="7">
         <v>1000</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B62" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C62" s="7">
         <v>175</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D62" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E45" s="7">
-        <v>512</v>
-      </c>
-      <c r="F45" s="8" t="s">
+      <c r="E62" s="7">
+        <v>512</v>
+      </c>
+      <c r="F62" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G62" s="7">
         <v>154</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H62" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="K45" s="10" t="s">
+      <c r="K62" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="L45" s="8" t="s">
+      <c r="L62" s="8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A46" s="7">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A63" s="7">
         <v>1000</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B63" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C63" s="7">
         <v>175</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D63" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="E46" s="7">
-        <v>512</v>
-      </c>
-      <c r="F46" s="8" t="s">
+      <c r="E63" s="7">
+        <v>512</v>
+      </c>
+      <c r="F63" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="I46" s="7">
+      <c r="I63" s="7">
         <v>2</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="J63" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="K46" s="10" t="s">
+      <c r="K63" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="L46" s="8" t="s">
+      <c r="L63" s="8" t="s">
         <v>183</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="G37:K37"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
evaluation metric for clustering algo
</commit_message>
<xml_diff>
--- a/Experiments/DBCV_Conclu.xlsx
+++ b/Experiments/DBCV_Conclu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18190" windowHeight="8510"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="196">
   <si>
     <t>Datapoints</t>
   </si>
@@ -585,18 +585,6 @@
     <t xml:space="preserve">Level 1 </t>
   </si>
   <si>
-    <t>298 clusters</t>
-  </si>
-  <si>
-    <t>95 outliers</t>
-  </si>
-  <si>
-    <t>0.141</t>
-  </si>
-  <si>
-    <t>225.495 secs</t>
-  </si>
-  <si>
     <t>Algo</t>
   </si>
   <si>
@@ -609,10 +597,25 @@
     <t>Level 2</t>
   </si>
   <si>
-    <t>-0.095</t>
-  </si>
-  <si>
-    <t>56.624 secs</t>
+    <t>309 clusters</t>
+  </si>
+  <si>
+    <t>86 outliers</t>
+  </si>
+  <si>
+    <t>0.151</t>
+  </si>
+  <si>
+    <t>244.744 secs</t>
+  </si>
+  <si>
+    <t>New Outliers</t>
+  </si>
+  <si>
+    <t>-0.055</t>
+  </si>
+  <si>
+    <t>54.398 secs</t>
   </si>
 </sst>
 </file>
@@ -1014,36 +1017,36 @@
   </sheetPr>
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="80.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="80.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G1" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1000</v>
       </c>
@@ -1123,7 +1126,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1000</v>
       </c>
@@ -1159,7 +1162,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1000</v>
       </c>
@@ -1195,7 +1198,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1000</v>
       </c>
@@ -1231,7 +1234,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1000</v>
       </c>
@@ -1267,7 +1270,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1000</v>
       </c>
@@ -1303,7 +1306,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1000</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1000</v>
       </c>
@@ -1379,7 +1382,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1392,7 +1395,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1405,7 +1408,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2000</v>
       </c>
@@ -1441,7 +1444,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>2000</v>
       </c>
@@ -1477,7 +1480,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2000</v>
       </c>
@@ -1515,7 +1518,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>2000</v>
       </c>
@@ -1551,7 +1554,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>2000</v>
       </c>
@@ -1587,7 +1590,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>2000</v>
       </c>
@@ -1623,7 +1626,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>2000</v>
       </c>
@@ -1659,7 +1662,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>2000</v>
       </c>
@@ -1695,7 +1698,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
@@ -1708,7 +1711,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
@@ -1721,7 +1724,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>5000</v>
       </c>
@@ -1757,7 +1760,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>5000</v>
       </c>
@@ -1795,7 +1798,7 @@
       </c>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>5000</v>
       </c>
@@ -1831,7 +1834,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>5000</v>
       </c>
@@ -1869,7 +1872,7 @@
       </c>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>5000</v>
       </c>
@@ -1905,7 +1908,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>5000</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>5000</v>
       </c>
@@ -1981,7 +1984,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>5000</v>
       </c>
@@ -2017,7 +2020,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
@@ -2033,7 +2036,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
@@ -2049,7 +2052,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
@@ -2065,7 +2068,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>102</v>
       </c>
@@ -2083,7 +2086,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
         <v>184</v>
       </c>
@@ -2092,22 +2095,22 @@
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>10</v>
@@ -2116,13 +2119,13 @@
         <v>11</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>10</v>
@@ -2131,7 +2134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>1000</v>
       </c>
@@ -2139,39 +2142,39 @@
         <v>14</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H39" s="8">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I39" s="7">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G54" s="9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>1000</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>1000</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>1000</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>1000</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>1000</v>
       </c>
@@ -2378,7 +2381,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>1000</v>
       </c>
@@ -2410,7 +2413,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>1000</v>
       </c>
@@ -2442,7 +2445,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>1000</v>
       </c>

</xml_diff>